<commit_message>
modified:   directorio_cuentas.xlsx modified:   model.py
</commit_message>
<xml_diff>
--- a/directorio_cuentas.xlsx
+++ b/directorio_cuentas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7617771dfdaae3ac/Documentos/Repositories/MIT_Tax_Avoidance/FTZ_Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="8_{E638D92E-5787-4DDD-B2F8-452135849A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{030E9039-1FAB-48F9-A1D6-DD43CE61AB1A}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="8_{E638D92E-5787-4DDD-B2F8-452135849A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{017FF27A-0672-43DC-9D35-331833C108E7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PUC" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2480" uniqueCount="1246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2481" uniqueCount="1247">
   <si>
     <t>Codigo</t>
   </si>
@@ -3772,6 +3772,9 @@
   </si>
   <si>
     <t>MERCANCIAS NO RELACIONADAS CON LA EMPRESA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integracion diagonal </t>
   </si>
 </sst>
 </file>
@@ -3961,16 +3964,16 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="thin">
+        <bottom style="thin">
           <color auto="1"/>
-        </top>
+        </bottom>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <top style="thin">
           <color auto="1"/>
-        </bottom>
+        </top>
       </border>
     </dxf>
     <dxf>
@@ -4016,10 +4019,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{039C9E28-7A82-4206-B833-F2027433125C}" name="Tabla1" displayName="Tabla1" ref="A1:E15" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
-  <autoFilter ref="A1:E15" xr:uid="{039C9E28-7A82-4206-B833-F2027433125C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E14">
-    <sortCondition descending="1" ref="A1:A14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{039C9E28-7A82-4206-B833-F2027433125C}" name="Tabla1" displayName="Tabla1" ref="A1:E16" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:E16" xr:uid="{039C9E28-7A82-4206-B833-F2027433125C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E15">
+    <sortCondition ref="A1:A15"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{A1C9C4D9-0D3E-4DEF-A209-E8D51D44BC3F}" name="codigo_cuenta"/>
@@ -4329,8 +4332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC9C66E-2E7F-4CAC-893E-A8AB04694B02}">
   <dimension ref="B1:C2481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A260" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C269" sqref="C269"/>
+    <sheetView topLeftCell="A2465" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2477" sqref="C2477"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -24132,6 +24135,14 @@
         <v>1238</v>
       </c>
     </row>
+    <row r="2476" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2476" s="2">
+        <v>9605</v>
+      </c>
+      <c r="C2476" s="2" t="s">
+        <v>1246</v>
+      </c>
+    </row>
     <row r="2479" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C2479" s="5"/>
     </row>
@@ -24146,10 +24157,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24180,296 +24191,317 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>6205</v>
+        <v>71</v>
       </c>
       <c r="B2" t="str">
         <f>_xlfn.CONCAT(VALUE(LEFT(A2,1))," ",VLOOKUP(VALUE(LEFT(A2,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>6 COSTOS DE VENTAS</v>
+        <v>7 COSTOS DE PRODUCCION O DE OPERACION</v>
       </c>
       <c r="C2" s="8">
-        <f t="shared" ref="C2:C14" si="0">+VALUE(LEFT(A2,1))</f>
-        <v>6</v>
+        <f>+VALUE(LEFT(A2,1))</f>
+        <v>7</v>
       </c>
       <c r="D2" t="str">
         <f>_xlfn.CONCAT(VALUE(LEFT(A2,2))," ",VLOOKUP(VALUE(LEFT(A2,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>71 MATERIA PRIMA</v>
+      </c>
+      <c r="E2" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B14:C2486,2,0)</f>
+        <v>MATERIA PRIMA</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>73</v>
+      </c>
+      <c r="B3" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A3,1))," ",VLOOKUP(VALUE(LEFT(A3,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>7 COSTOS DE PRODUCCION O DE OPERACION</v>
+      </c>
+      <c r="C3" s="8">
+        <f>+VALUE(LEFT(A3,1))</f>
+        <v>7</v>
+      </c>
+      <c r="D3" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A3,2))," ",VLOOKUP(VALUE(LEFT(A3,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>73 COSTOS INDIRECTOS</v>
+      </c>
+      <c r="E3" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B15:C2487,2,0)</f>
+        <v>COSTOS INDIRECTOS</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1105</v>
+      </c>
+      <c r="B4" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A4,1))," ",VLOOKUP(VALUE(LEFT(A4,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>1 ACTIVO</v>
+      </c>
+      <c r="C4" s="8">
+        <f>+VALUE(LEFT(A4,1))</f>
+        <v>1</v>
+      </c>
+      <c r="D4" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A4,2))," ",VLOOKUP(VALUE(LEFT(A4,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>11 DISPONIBLE</v>
+      </c>
+      <c r="E4" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B3:C2475,2,0)</f>
+        <v>CAJA</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1405</v>
+      </c>
+      <c r="B5" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A5,1))," ",VLOOKUP(VALUE(LEFT(A5,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>1 ACTIVO</v>
+      </c>
+      <c r="C5" s="8">
+        <f>+VALUE(LEFT(A5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="D5" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A5,2))," ",VLOOKUP(VALUE(LEFT(A5,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>14 INVENTARIOS</v>
+      </c>
+      <c r="E5" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B4:C2476,2,0)</f>
+        <v>MATERIAS PRIMAS</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1411</v>
+      </c>
+      <c r="B6" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A6,1))," ",VLOOKUP(VALUE(LEFT(A6,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>1 ACTIVO</v>
+      </c>
+      <c r="C6" s="8">
+        <f>+VALUE(LEFT(A6,1))</f>
+        <v>1</v>
+      </c>
+      <c r="D6" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A6,2))," ",VLOOKUP(VALUE(LEFT(A6,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>14 INVENTARIOS</v>
+      </c>
+      <c r="E6" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B16:C2488,2,0)</f>
+        <v>MERCANCIAS NO RELACIONADAS CON LA EMPRESA</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1430</v>
+      </c>
+      <c r="B7" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A7,1))," ",VLOOKUP(VALUE(LEFT(A7,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>1 ACTIVO</v>
+      </c>
+      <c r="C7" s="8">
+        <f>+VALUE(LEFT(A7,1))</f>
+        <v>1</v>
+      </c>
+      <c r="D7" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A7,2))," ",VLOOKUP(VALUE(LEFT(A7,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>14 INVENTARIOS</v>
+      </c>
+      <c r="E7" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B5:C2477,2,0)</f>
+        <v>PRODUCTOS TERMINADOS</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1435</v>
+      </c>
+      <c r="B8" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A8,1))," ",VLOOKUP(VALUE(LEFT(A8,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>1 ACTIVO</v>
+      </c>
+      <c r="C8" s="8">
+        <f>+VALUE(LEFT(A8,1))</f>
+        <v>1</v>
+      </c>
+      <c r="D8" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A8,2))," ",VLOOKUP(VALUE(LEFT(A8,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>14 INVENTARIOS</v>
+      </c>
+      <c r="E8" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B6:C2478,2,0)</f>
+        <v>MERCANCIAS NO FABRICADAS POR LA EMPRESA</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2408</v>
+      </c>
+      <c r="B9" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A9,1))," ",VLOOKUP(VALUE(LEFT(A9,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>2 PASIVO</v>
+      </c>
+      <c r="C9" s="8">
+        <f>+VALUE(LEFT(A9,1))</f>
+        <v>2</v>
+      </c>
+      <c r="D9" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A9,2))," ",VLOOKUP(VALUE(LEFT(A9,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>24 IMPUESTOS, GRAVAMENES Y TASAS</v>
+      </c>
+      <c r="E9" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B7:C2479,2,0)</f>
+        <v>IMPUESTO SOBRE LAS VENTAS POR PAGAR</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3115</v>
+      </c>
+      <c r="B10" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A10,1))," ",VLOOKUP(VALUE(LEFT(A10,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>3 PATRIMONIO</v>
+      </c>
+      <c r="C10" s="8">
+        <f>+VALUE(LEFT(A10,1))</f>
+        <v>3</v>
+      </c>
+      <c r="D10" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A10,2))," ",VLOOKUP(VALUE(LEFT(A10,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>31 CAPITAL SOCIAL</v>
+      </c>
+      <c r="E10" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B8:C2480,2,0)</f>
+        <v>APORTES SOCIALES</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4120</v>
+      </c>
+      <c r="B11" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A11,1))," ",VLOOKUP(VALUE(LEFT(A11,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>4 INGRESOS</v>
+      </c>
+      <c r="C11" s="8">
+        <f>+VALUE(LEFT(A11,1))</f>
+        <v>4</v>
+      </c>
+      <c r="D11" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A11,2))," ",VLOOKUP(VALUE(LEFT(A11,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>41 OPERACIONALES</v>
+      </c>
+      <c r="E11" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B9:C2481,2,0)</f>
+        <v>INDUSTRIAS MANUFACTURERAS</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4135</v>
+      </c>
+      <c r="B12" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A12,1))," ",VLOOKUP(VALUE(LEFT(A12,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>4 INGRESOS</v>
+      </c>
+      <c r="C12" s="8">
+        <f>+VALUE(LEFT(A12,1))</f>
+        <v>4</v>
+      </c>
+      <c r="D12" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A12,2))," ",VLOOKUP(VALUE(LEFT(A12,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>41 OPERACIONALES</v>
+      </c>
+      <c r="E12" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B10:C2482,2,0)</f>
+        <v>COMERCIO AL POR MAYOR Y AL POR MENOR</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>6120</v>
+      </c>
+      <c r="B13" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A13,1))," ",VLOOKUP(VALUE(LEFT(A13,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>6 COSTOS DE VENTAS</v>
+      </c>
+      <c r="C13" s="8">
+        <f>+VALUE(LEFT(A13,1))</f>
+        <v>6</v>
+      </c>
+      <c r="D13" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A13,2))," ",VLOOKUP(VALUE(LEFT(A13,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>61 COSTO DE VENTAS Y DE PRESTACION DE SERVICIOS</v>
+      </c>
+      <c r="E13" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B11:C2483,2,0)</f>
+        <v>INDUSTRIAS MANUFACTURERAS</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6135</v>
+      </c>
+      <c r="B14" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A14,1))," ",VLOOKUP(VALUE(LEFT(A14,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>6 COSTOS DE VENTAS</v>
+      </c>
+      <c r="C14" s="8">
+        <f>+VALUE(LEFT(A14,1))</f>
+        <v>6</v>
+      </c>
+      <c r="D14" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A14,2))," ",VLOOKUP(VALUE(LEFT(A14,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>61 COSTO DE VENTAS Y DE PRESTACION DE SERVICIOS</v>
+      </c>
+      <c r="E14" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B12:C2484,2,0)</f>
+        <v>COMERCIO AL POR MAYOR Y AL POR MENOR</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>6205</v>
+      </c>
+      <c r="B15" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A15,1))," ",VLOOKUP(VALUE(LEFT(A15,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>6 COSTOS DE VENTAS</v>
+      </c>
+      <c r="C15" s="8">
+        <f>+VALUE(LEFT(A15,1))</f>
+        <v>6</v>
+      </c>
+      <c r="D15" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A15,2))," ",VLOOKUP(VALUE(LEFT(A15,2)),PUC!$B$3:$C$2475,2,0))</f>
         <v>62 COMPRAS</v>
       </c>
-      <c r="E2" t="str">
+      <c r="E15" t="str">
         <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B13:C2485,2,0)</f>
         <v>COMPRAS DE MERCANCIAS</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>6135</v>
-      </c>
-      <c r="B3" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A3,1))," ",VLOOKUP(VALUE(LEFT(A3,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>6 COSTOS DE VENTAS</v>
-      </c>
-      <c r="C3" s="8">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="D3" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A3,2))," ",VLOOKUP(VALUE(LEFT(A3,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>61 COSTO DE VENTAS Y DE PRESTACION DE SERVICIOS</v>
-      </c>
-      <c r="E3" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B12:C2484,2,0)</f>
-        <v>COMERCIO AL POR MAYOR Y AL POR MENOR</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>6120</v>
-      </c>
-      <c r="B4" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A4,1))," ",VLOOKUP(VALUE(LEFT(A4,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>6 COSTOS DE VENTAS</v>
-      </c>
-      <c r="C4" s="8">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="D4" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A4,2))," ",VLOOKUP(VALUE(LEFT(A4,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>61 COSTO DE VENTAS Y DE PRESTACION DE SERVICIOS</v>
-      </c>
-      <c r="E4" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B11:C2483,2,0)</f>
-        <v>INDUSTRIAS MANUFACTURERAS</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4135</v>
-      </c>
-      <c r="B5" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A5,1))," ",VLOOKUP(VALUE(LEFT(A5,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>4 INGRESOS</v>
-      </c>
-      <c r="C5" s="8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="D5" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A5,2))," ",VLOOKUP(VALUE(LEFT(A5,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>41 OPERACIONALES</v>
-      </c>
-      <c r="E5" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B10:C2482,2,0)</f>
-        <v>COMERCIO AL POR MAYOR Y AL POR MENOR</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4120</v>
-      </c>
-      <c r="B6" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A6,1))," ",VLOOKUP(VALUE(LEFT(A6,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>4 INGRESOS</v>
-      </c>
-      <c r="C6" s="8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="D6" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A6,2))," ",VLOOKUP(VALUE(LEFT(A6,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>41 OPERACIONALES</v>
-      </c>
-      <c r="E6" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B9:C2481,2,0)</f>
-        <v>INDUSTRIAS MANUFACTURERAS</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3115</v>
-      </c>
-      <c r="B7" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A7,1))," ",VLOOKUP(VALUE(LEFT(A7,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>3 PATRIMONIO</v>
-      </c>
-      <c r="C7" s="8">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D7" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A7,2))," ",VLOOKUP(VALUE(LEFT(A7,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>31 CAPITAL SOCIAL</v>
-      </c>
-      <c r="E7" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B8:C2480,2,0)</f>
-        <v>APORTES SOCIALES</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2408</v>
-      </c>
-      <c r="B8" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A8,1))," ",VLOOKUP(VALUE(LEFT(A8,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>2 PASIVO</v>
-      </c>
-      <c r="C8" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D8" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A8,2))," ",VLOOKUP(VALUE(LEFT(A8,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>24 IMPUESTOS, GRAVAMENES Y TASAS</v>
-      </c>
-      <c r="E8" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B7:C2479,2,0)</f>
-        <v>IMPUESTO SOBRE LAS VENTAS POR PAGAR</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1435</v>
-      </c>
-      <c r="B9" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A9,1))," ",VLOOKUP(VALUE(LEFT(A9,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>1 ACTIVO</v>
-      </c>
-      <c r="C9" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D9" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A9,2))," ",VLOOKUP(VALUE(LEFT(A9,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>14 INVENTARIOS</v>
-      </c>
-      <c r="E9" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B6:C2478,2,0)</f>
-        <v>MERCANCIAS NO FABRICADAS POR LA EMPRESA</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1430</v>
-      </c>
-      <c r="B10" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A10,1))," ",VLOOKUP(VALUE(LEFT(A10,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>1 ACTIVO</v>
-      </c>
-      <c r="C10" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D10" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A10,2))," ",VLOOKUP(VALUE(LEFT(A10,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>14 INVENTARIOS</v>
-      </c>
-      <c r="E10" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B5:C2477,2,0)</f>
-        <v>PRODUCTOS TERMINADOS</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1405</v>
-      </c>
-      <c r="B11" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A11,1))," ",VLOOKUP(VALUE(LEFT(A11,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>1 ACTIVO</v>
-      </c>
-      <c r="C11" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D11" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A11,2))," ",VLOOKUP(VALUE(LEFT(A11,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>14 INVENTARIOS</v>
-      </c>
-      <c r="E11" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B4:C2476,2,0)</f>
-        <v>MATERIAS PRIMAS</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1105</v>
-      </c>
-      <c r="B12" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A12,1))," ",VLOOKUP(VALUE(LEFT(A12,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>1 ACTIVO</v>
-      </c>
-      <c r="C12" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D12" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A12,2))," ",VLOOKUP(VALUE(LEFT(A12,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>11 DISPONIBLE</v>
-      </c>
-      <c r="E12" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B3:C2475,2,0)</f>
-        <v>CAJA</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>73</v>
-      </c>
-      <c r="B13" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A13,1))," ",VLOOKUP(VALUE(LEFT(A13,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>7 COSTOS DE PRODUCCION O DE OPERACION</v>
-      </c>
-      <c r="C13" s="8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="D13" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A13,2))," ",VLOOKUP(VALUE(LEFT(A13,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>73 COSTOS INDIRECTOS</v>
-      </c>
-      <c r="E13" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B15:C2487,2,0)</f>
-        <v>COSTOS INDIRECTOS</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>71</v>
-      </c>
-      <c r="B14" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A14,1))," ",VLOOKUP(VALUE(LEFT(A14,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>7 COSTOS DE PRODUCCION O DE OPERACION</v>
-      </c>
-      <c r="C14" s="8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="D14" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A14,2))," ",VLOOKUP(VALUE(LEFT(A14,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>71 MATERIA PRIMA</v>
-      </c>
-      <c r="E14" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B14:C2486,2,0)</f>
-        <v>MATERIA PRIMA</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1411</v>
-      </c>
-      <c r="B15" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A15,1))," ",VLOOKUP(VALUE(LEFT(A15,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>1 ACTIVO</v>
-      </c>
-      <c r="C15" s="9">
-        <f>+VALUE(LEFT(A15,1))</f>
-        <v>1</v>
-      </c>
-      <c r="D15" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A15,2))," ",VLOOKUP(VALUE(LEFT(A15,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>14 INVENTARIOS</v>
-      </c>
-      <c r="E15" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B16:C2488,2,0)</f>
-        <v>MERCANCIAS NO RELACIONADAS CON LA EMPRESA</v>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>9605</v>
+      </c>
+      <c r="B16" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A16,1))," ",VLOOKUP(VALUE(LEFT(A16,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>9 CUENTAS DE ORDEN ACREEDORAS</v>
+      </c>
+      <c r="C16" s="9">
+        <f>+VALUE(LEFT(A16,1))</f>
+        <v>9</v>
+      </c>
+      <c r="D16" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A16,2))," ",VLOOKUP(VALUE(LEFT(A16,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>96 ACREEDORAS DE CONTROL POR CONTRA (DB)</v>
+      </c>
+      <c r="E16" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B17:C2489,2,0)</f>
+        <v xml:space="preserve">Integracion diagonal </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   classes.py modified:   directorio_cuentas.xlsx modified:   test.py modified:   utils.py
</commit_message>
<xml_diff>
--- a/directorio_cuentas.xlsx
+++ b/directorio_cuentas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7617771dfdaae3ac/Documentos/Repositories/MIT_Tax_Avoidance/FTZ_Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="8_{E638D92E-5787-4DDD-B2F8-452135849A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{030E9039-1FAB-48F9-A1D6-DD43CE61AB1A}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="8_{E638D92E-5787-4DDD-B2F8-452135849A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{017FF27A-0672-43DC-9D35-331833C108E7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PUC" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2480" uniqueCount="1246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2481" uniqueCount="1247">
   <si>
     <t>Codigo</t>
   </si>
@@ -3772,6 +3772,9 @@
   </si>
   <si>
     <t>MERCANCIAS NO RELACIONADAS CON LA EMPRESA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integracion diagonal </t>
   </si>
 </sst>
 </file>
@@ -3920,7 +3923,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3942,9 +3945,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4016,10 +4016,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{039C9E28-7A82-4206-B833-F2027433125C}" name="Tabla1" displayName="Tabla1" ref="A1:E15" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
-  <autoFilter ref="A1:E15" xr:uid="{039C9E28-7A82-4206-B833-F2027433125C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E14">
-    <sortCondition descending="1" ref="A1:A14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{039C9E28-7A82-4206-B833-F2027433125C}" name="Tabla1" displayName="Tabla1" ref="A1:E16" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="A1:E16" xr:uid="{039C9E28-7A82-4206-B833-F2027433125C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E15">
+    <sortCondition ref="A1:A15"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{A1C9C4D9-0D3E-4DEF-A209-E8D51D44BC3F}" name="codigo_cuenta"/>
@@ -4329,8 +4329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC9C66E-2E7F-4CAC-893E-A8AB04694B02}">
   <dimension ref="B1:C2481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A260" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C269" sqref="C269"/>
+    <sheetView topLeftCell="A2465" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2477" sqref="C2477"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -24132,6 +24132,14 @@
         <v>1238</v>
       </c>
     </row>
+    <row r="2476" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2476" s="2">
+        <v>9605</v>
+      </c>
+      <c r="C2476" s="2" t="s">
+        <v>1246</v>
+      </c>
+    </row>
     <row r="2479" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C2479" s="5"/>
     </row>
@@ -24146,10 +24154,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24180,296 +24188,317 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>6205</v>
+        <v>71</v>
       </c>
       <c r="B2" t="str">
         <f>_xlfn.CONCAT(VALUE(LEFT(A2,1))," ",VLOOKUP(VALUE(LEFT(A2,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>6 COSTOS DE VENTAS</v>
+        <v>7 COSTOS DE PRODUCCION O DE OPERACION</v>
       </c>
       <c r="C2" s="8">
-        <f t="shared" ref="C2:C14" si="0">+VALUE(LEFT(A2,1))</f>
-        <v>6</v>
+        <f t="shared" ref="C2:C16" si="0">+VALUE(LEFT(A2,1))</f>
+        <v>7</v>
       </c>
       <c r="D2" t="str">
         <f>_xlfn.CONCAT(VALUE(LEFT(A2,2))," ",VLOOKUP(VALUE(LEFT(A2,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>71 MATERIA PRIMA</v>
+      </c>
+      <c r="E2" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B14:C2486,2,0)</f>
+        <v>MATERIA PRIMA</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>73</v>
+      </c>
+      <c r="B3" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A3,1))," ",VLOOKUP(VALUE(LEFT(A3,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>7 COSTOS DE PRODUCCION O DE OPERACION</v>
+      </c>
+      <c r="C3" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D3" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A3,2))," ",VLOOKUP(VALUE(LEFT(A3,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>73 COSTOS INDIRECTOS</v>
+      </c>
+      <c r="E3" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B15:C2487,2,0)</f>
+        <v>COSTOS INDIRECTOS</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1105</v>
+      </c>
+      <c r="B4" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A4,1))," ",VLOOKUP(VALUE(LEFT(A4,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>1 ACTIVO</v>
+      </c>
+      <c r="C4" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D4" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A4,2))," ",VLOOKUP(VALUE(LEFT(A4,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>11 DISPONIBLE</v>
+      </c>
+      <c r="E4" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B3:C2475,2,0)</f>
+        <v>CAJA</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1405</v>
+      </c>
+      <c r="B5" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A5,1))," ",VLOOKUP(VALUE(LEFT(A5,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>1 ACTIVO</v>
+      </c>
+      <c r="C5" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D5" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A5,2))," ",VLOOKUP(VALUE(LEFT(A5,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>14 INVENTARIOS</v>
+      </c>
+      <c r="E5" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B4:C2476,2,0)</f>
+        <v>MATERIAS PRIMAS</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1411</v>
+      </c>
+      <c r="B6" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A6,1))," ",VLOOKUP(VALUE(LEFT(A6,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>1 ACTIVO</v>
+      </c>
+      <c r="C6" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D6" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A6,2))," ",VLOOKUP(VALUE(LEFT(A6,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>14 INVENTARIOS</v>
+      </c>
+      <c r="E6" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B16:C2488,2,0)</f>
+        <v>MERCANCIAS NO RELACIONADAS CON LA EMPRESA</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1430</v>
+      </c>
+      <c r="B7" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A7,1))," ",VLOOKUP(VALUE(LEFT(A7,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>1 ACTIVO</v>
+      </c>
+      <c r="C7" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D7" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A7,2))," ",VLOOKUP(VALUE(LEFT(A7,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>14 INVENTARIOS</v>
+      </c>
+      <c r="E7" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B5:C2477,2,0)</f>
+        <v>PRODUCTOS TERMINADOS</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1435</v>
+      </c>
+      <c r="B8" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A8,1))," ",VLOOKUP(VALUE(LEFT(A8,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>1 ACTIVO</v>
+      </c>
+      <c r="C8" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D8" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A8,2))," ",VLOOKUP(VALUE(LEFT(A8,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>14 INVENTARIOS</v>
+      </c>
+      <c r="E8" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B6:C2478,2,0)</f>
+        <v>MERCANCIAS NO FABRICADAS POR LA EMPRESA</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2408</v>
+      </c>
+      <c r="B9" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A9,1))," ",VLOOKUP(VALUE(LEFT(A9,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>2 PASIVO</v>
+      </c>
+      <c r="C9" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D9" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A9,2))," ",VLOOKUP(VALUE(LEFT(A9,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>24 IMPUESTOS, GRAVAMENES Y TASAS</v>
+      </c>
+      <c r="E9" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B7:C2479,2,0)</f>
+        <v>IMPUESTO SOBRE LAS VENTAS POR PAGAR</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3115</v>
+      </c>
+      <c r="B10" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A10,1))," ",VLOOKUP(VALUE(LEFT(A10,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>3 PATRIMONIO</v>
+      </c>
+      <c r="C10" s="8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D10" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A10,2))," ",VLOOKUP(VALUE(LEFT(A10,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>31 CAPITAL SOCIAL</v>
+      </c>
+      <c r="E10" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B8:C2480,2,0)</f>
+        <v>APORTES SOCIALES</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4120</v>
+      </c>
+      <c r="B11" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A11,1))," ",VLOOKUP(VALUE(LEFT(A11,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>4 INGRESOS</v>
+      </c>
+      <c r="C11" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D11" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A11,2))," ",VLOOKUP(VALUE(LEFT(A11,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>41 OPERACIONALES</v>
+      </c>
+      <c r="E11" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B9:C2481,2,0)</f>
+        <v>INDUSTRIAS MANUFACTURERAS</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4135</v>
+      </c>
+      <c r="B12" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A12,1))," ",VLOOKUP(VALUE(LEFT(A12,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>4 INGRESOS</v>
+      </c>
+      <c r="C12" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D12" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A12,2))," ",VLOOKUP(VALUE(LEFT(A12,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>41 OPERACIONALES</v>
+      </c>
+      <c r="E12" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B10:C2482,2,0)</f>
+        <v>COMERCIO AL POR MAYOR Y AL POR MENOR</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>6120</v>
+      </c>
+      <c r="B13" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A13,1))," ",VLOOKUP(VALUE(LEFT(A13,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>6 COSTOS DE VENTAS</v>
+      </c>
+      <c r="C13" s="8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D13" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A13,2))," ",VLOOKUP(VALUE(LEFT(A13,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>61 COSTO DE VENTAS Y DE PRESTACION DE SERVICIOS</v>
+      </c>
+      <c r="E13" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B11:C2483,2,0)</f>
+        <v>INDUSTRIAS MANUFACTURERAS</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6135</v>
+      </c>
+      <c r="B14" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A14,1))," ",VLOOKUP(VALUE(LEFT(A14,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>6 COSTOS DE VENTAS</v>
+      </c>
+      <c r="C14" s="8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D14" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A14,2))," ",VLOOKUP(VALUE(LEFT(A14,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>61 COSTO DE VENTAS Y DE PRESTACION DE SERVICIOS</v>
+      </c>
+      <c r="E14" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B12:C2484,2,0)</f>
+        <v>COMERCIO AL POR MAYOR Y AL POR MENOR</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>6205</v>
+      </c>
+      <c r="B15" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A15,1))," ",VLOOKUP(VALUE(LEFT(A15,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>6 COSTOS DE VENTAS</v>
+      </c>
+      <c r="C15" s="8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D15" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A15,2))," ",VLOOKUP(VALUE(LEFT(A15,2)),PUC!$B$3:$C$2475,2,0))</f>
         <v>62 COMPRAS</v>
       </c>
-      <c r="E2" t="str">
+      <c r="E15" t="str">
         <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B13:C2485,2,0)</f>
         <v>COMPRAS DE MERCANCIAS</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>6135</v>
-      </c>
-      <c r="B3" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A3,1))," ",VLOOKUP(VALUE(LEFT(A3,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>6 COSTOS DE VENTAS</v>
-      </c>
-      <c r="C3" s="8">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>9605</v>
+      </c>
+      <c r="B16" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A16,1))," ",VLOOKUP(VALUE(LEFT(A16,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>9 CUENTAS DE ORDEN ACREEDORAS</v>
+      </c>
+      <c r="C16" s="8">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="D3" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A3,2))," ",VLOOKUP(VALUE(LEFT(A3,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>61 COSTO DE VENTAS Y DE PRESTACION DE SERVICIOS</v>
-      </c>
-      <c r="E3" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B12:C2484,2,0)</f>
-        <v>COMERCIO AL POR MAYOR Y AL POR MENOR</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>6120</v>
-      </c>
-      <c r="B4" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A4,1))," ",VLOOKUP(VALUE(LEFT(A4,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>6 COSTOS DE VENTAS</v>
-      </c>
-      <c r="C4" s="8">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="D4" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A4,2))," ",VLOOKUP(VALUE(LEFT(A4,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>61 COSTO DE VENTAS Y DE PRESTACION DE SERVICIOS</v>
-      </c>
-      <c r="E4" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B11:C2483,2,0)</f>
-        <v>INDUSTRIAS MANUFACTURERAS</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4135</v>
-      </c>
-      <c r="B5" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A5,1))," ",VLOOKUP(VALUE(LEFT(A5,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>4 INGRESOS</v>
-      </c>
-      <c r="C5" s="8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="D5" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A5,2))," ",VLOOKUP(VALUE(LEFT(A5,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>41 OPERACIONALES</v>
-      </c>
-      <c r="E5" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B10:C2482,2,0)</f>
-        <v>COMERCIO AL POR MAYOR Y AL POR MENOR</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4120</v>
-      </c>
-      <c r="B6" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A6,1))," ",VLOOKUP(VALUE(LEFT(A6,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>4 INGRESOS</v>
-      </c>
-      <c r="C6" s="8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="D6" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A6,2))," ",VLOOKUP(VALUE(LEFT(A6,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>41 OPERACIONALES</v>
-      </c>
-      <c r="E6" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B9:C2481,2,0)</f>
-        <v>INDUSTRIAS MANUFACTURERAS</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3115</v>
-      </c>
-      <c r="B7" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A7,1))," ",VLOOKUP(VALUE(LEFT(A7,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>3 PATRIMONIO</v>
-      </c>
-      <c r="C7" s="8">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D7" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A7,2))," ",VLOOKUP(VALUE(LEFT(A7,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>31 CAPITAL SOCIAL</v>
-      </c>
-      <c r="E7" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B8:C2480,2,0)</f>
-        <v>APORTES SOCIALES</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2408</v>
-      </c>
-      <c r="B8" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A8,1))," ",VLOOKUP(VALUE(LEFT(A8,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>2 PASIVO</v>
-      </c>
-      <c r="C8" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D8" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A8,2))," ",VLOOKUP(VALUE(LEFT(A8,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>24 IMPUESTOS, GRAVAMENES Y TASAS</v>
-      </c>
-      <c r="E8" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B7:C2479,2,0)</f>
-        <v>IMPUESTO SOBRE LAS VENTAS POR PAGAR</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1435</v>
-      </c>
-      <c r="B9" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A9,1))," ",VLOOKUP(VALUE(LEFT(A9,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>1 ACTIVO</v>
-      </c>
-      <c r="C9" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D9" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A9,2))," ",VLOOKUP(VALUE(LEFT(A9,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>14 INVENTARIOS</v>
-      </c>
-      <c r="E9" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B6:C2478,2,0)</f>
-        <v>MERCANCIAS NO FABRICADAS POR LA EMPRESA</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1430</v>
-      </c>
-      <c r="B10" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A10,1))," ",VLOOKUP(VALUE(LEFT(A10,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>1 ACTIVO</v>
-      </c>
-      <c r="C10" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D10" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A10,2))," ",VLOOKUP(VALUE(LEFT(A10,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>14 INVENTARIOS</v>
-      </c>
-      <c r="E10" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B5:C2477,2,0)</f>
-        <v>PRODUCTOS TERMINADOS</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1405</v>
-      </c>
-      <c r="B11" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A11,1))," ",VLOOKUP(VALUE(LEFT(A11,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>1 ACTIVO</v>
-      </c>
-      <c r="C11" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D11" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A11,2))," ",VLOOKUP(VALUE(LEFT(A11,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>14 INVENTARIOS</v>
-      </c>
-      <c r="E11" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B4:C2476,2,0)</f>
-        <v>MATERIAS PRIMAS</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1105</v>
-      </c>
-      <c r="B12" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A12,1))," ",VLOOKUP(VALUE(LEFT(A12,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>1 ACTIVO</v>
-      </c>
-      <c r="C12" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D12" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A12,2))," ",VLOOKUP(VALUE(LEFT(A12,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>11 DISPONIBLE</v>
-      </c>
-      <c r="E12" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B3:C2475,2,0)</f>
-        <v>CAJA</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>73</v>
-      </c>
-      <c r="B13" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A13,1))," ",VLOOKUP(VALUE(LEFT(A13,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>7 COSTOS DE PRODUCCION O DE OPERACION</v>
-      </c>
-      <c r="C13" s="8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="D13" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A13,2))," ",VLOOKUP(VALUE(LEFT(A13,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>73 COSTOS INDIRECTOS</v>
-      </c>
-      <c r="E13" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B15:C2487,2,0)</f>
-        <v>COSTOS INDIRECTOS</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>71</v>
-      </c>
-      <c r="B14" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A14,1))," ",VLOOKUP(VALUE(LEFT(A14,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>7 COSTOS DE PRODUCCION O DE OPERACION</v>
-      </c>
-      <c r="C14" s="8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="D14" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A14,2))," ",VLOOKUP(VALUE(LEFT(A14,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>71 MATERIA PRIMA</v>
-      </c>
-      <c r="E14" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B14:C2486,2,0)</f>
-        <v>MATERIA PRIMA</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1411</v>
-      </c>
-      <c r="B15" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A15,1))," ",VLOOKUP(VALUE(LEFT(A15,1)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>1 ACTIVO</v>
-      </c>
-      <c r="C15" s="9">
-        <f>+VALUE(LEFT(A15,1))</f>
-        <v>1</v>
-      </c>
-      <c r="D15" t="str">
-        <f>_xlfn.CONCAT(VALUE(LEFT(A15,2))," ",VLOOKUP(VALUE(LEFT(A15,2)),PUC!$B$3:$C$2475,2,0))</f>
-        <v>14 INVENTARIOS</v>
-      </c>
-      <c r="E15" t="str">
-        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B16:C2488,2,0)</f>
-        <v>MERCANCIAS NO RELACIONADAS CON LA EMPRESA</v>
+        <v>9</v>
+      </c>
+      <c r="D16" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A16,2))," ",VLOOKUP(VALUE(LEFT(A16,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>96 ACREEDORAS DE CONTROL POR CONTRA (DB)</v>
+      </c>
+      <c r="E16" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B17:C2489,2,0)</f>
+        <v xml:space="preserve">Integracion diagonal </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   __pycache__/accounting_templates.cpython-311.pyc 	modified:   __pycache__/classes.cpython-311.pyc 	new file:   __pycache__/search_loop.cpython-311.pyc 	modified:   accounting_templates.py 	modified:   classes.py 	modified:   directorio_cuentas.xlsx 	new file:   search_loop.py 	new file:   simulation.ipynb 	deleted:    test.py
</commit_message>
<xml_diff>
--- a/directorio_cuentas.xlsx
+++ b/directorio_cuentas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7617771dfdaae3ac/Documentos/Repositories/MIT_Tax_Avoidance/FTZ_Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="8_{E638D92E-5787-4DDD-B2F8-452135849A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{017FF27A-0672-43DC-9D35-331833C108E7}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="8_{E638D92E-5787-4DDD-B2F8-452135849A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B571305-B88C-439D-9DA4-B7BA7D6281F3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3781,7 +3781,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3840,6 +3840,14 @@
       <color indexed="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -3923,7 +3931,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3947,6 +3955,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8"/>
@@ -4016,8 +4025,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{039C9E28-7A82-4206-B833-F2027433125C}" name="Tabla1" displayName="Tabla1" ref="A1:E16" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
-  <autoFilter ref="A1:E16" xr:uid="{039C9E28-7A82-4206-B833-F2027433125C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{039C9E28-7A82-4206-B833-F2027433125C}" name="Tabla1" displayName="Tabla1" ref="A1:E17" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="A1:E17" xr:uid="{039C9E28-7A82-4206-B833-F2027433125C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E15">
     <sortCondition ref="A1:A15"/>
   </sortState>
@@ -24154,10 +24163,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24501,6 +24510,30 @@
         <v xml:space="preserve">Integracion diagonal </v>
       </c>
     </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1410</v>
+      </c>
+      <c r="B17" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A17,1))," ",VLOOKUP(VALUE(LEFT(A17,1)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>1 ACTIVO</v>
+      </c>
+      <c r="C17" s="8">
+        <f>+VALUE(LEFT(A17,1))</f>
+        <v>1</v>
+      </c>
+      <c r="D17" t="str">
+        <f>_xlfn.CONCAT(VALUE(LEFT(A17,2))," ",VLOOKUP(VALUE(LEFT(A17,2)),PUC!$B$3:$C$2475,2,0))</f>
+        <v>14 INVENTARIOS</v>
+      </c>
+      <c r="E17" t="str">
+        <f>+VLOOKUP(Tabla1[[#This Row],[codigo_cuenta]],PUC!B18:C2490,2,0)</f>
+        <v>PRODUCTOS EN PROCESO</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>